<commit_message>
Primera Refactorizacion Cobranza por Cabeceras
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Cobranza por Prestaciones/Cobranza por Cabeceras/parametros_servidor.xlsx
+++ b/DBA/Reportes BI/2021/Cobranza por Prestaciones/Cobranza por Cabeceras/parametros_servidor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Efectores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Cobranza por Prestaciones\Cobranza por Cabeceras\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,13 +80,13 @@
     <t>serveradmin</t>
   </si>
   <si>
-    <t>facoep</t>
-  </si>
-  <si>
     <t>E:/Personales/Sistemas/Agustin/Reportes BI/2021/Efectores</t>
   </si>
   <si>
     <t>C:/Users/iachenbach/Gobierno de la Ciudad de Buenos Aires/Pablo Alfredo Gadea - Tablero Facoep P BI/FACOEP/DBA/Reportes BI/2021/Efectores</t>
+  </si>
+  <si>
+    <t>facoep1</t>
   </si>
 </sst>
 </file>
@@ -150,7 +150,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C14" totalsRowShown="0">
-  <autoFilter ref="A1:C14"/>
+  <autoFilter ref="A1:C14">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="password"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" name="Parametros servidor"/>
     <tableColumn id="2" name="Valor"/>
@@ -425,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -454,10 +460,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -465,7 +471,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -476,32 +482,32 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -512,7 +518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -534,18 +540,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -553,10 +559,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -564,10 +570,10 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -575,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -586,7 +592,7 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>